<commit_message>
Few things has been changed
</commit_message>
<xml_diff>
--- a/Leet Code Problems Takeaways.xlsx
+++ b/Leet Code Problems Takeaways.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,20 +26,20 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Prooblem Number</t>
-  </si>
-  <si>
     <t>Approach</t>
   </si>
   <si>
     <t>Key Takeaways</t>
+  </si>
+  <si>
+    <t>Problem Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,16 +47,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -64,12 +90,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,28 +401,30 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Few changes are made in Excel Sheet
</commit_message>
<xml_diff>
--- a/Leet Code Problems Takeaways.xlsx
+++ b/Leet Code Problems Takeaways.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Approach</t>
   </si>
@@ -32,14 +32,35 @@
     <t>Key Takeaways</t>
   </si>
   <si>
-    <t>Problem Number</t>
+    <t>Date Solved</t>
+  </si>
+  <si>
+    <t>Problem Name</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Time Complexity</t>
+  </si>
+  <si>
+    <t>Space Complexity</t>
+  </si>
+  <si>
+    <t>Mistakes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,8 +76,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,13 +100,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -106,20 +171,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,30 +528,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="27" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="30" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="7" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>